<commit_message>
12 Oct results update
</commit_message>
<xml_diff>
--- a/public/bowling_weekly_scores.xlsx
+++ b/public/bowling_weekly_scores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8675"/>
+    <workbookView windowWidth="23040" windowHeight="9120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Stats" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>Bowler</t>
   </si>
@@ -820,7 +820,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -850,12 +850,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="181" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="181" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="180" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1182,12 +1186,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1221,20 +1225,20 @@
         <v>5</v>
       </c>
       <c r="B2" s="12">
-        <f>AVERAGE(B10:B14,B16:B20,B21,B23:B28,B30:B36,B38:B42)</f>
-        <v>93.0344827586207</v>
+        <f>AVERAGE(B10:B14,B16:B20,B21,B23:B28,B30:B36,B38:B42,B45:B50)</f>
+        <v>94.3714285714286</v>
       </c>
       <c r="C2" s="12">
-        <f>AVERAGE(C10:C14,C16:C20,C21,C23:C28,C30:C36,C38:C43)</f>
-        <v>110.4</v>
+        <f>AVERAGE(C10:C14,C16:C20,C21,C23:C28,C30:C36,C38:C43,C45:C50)</f>
+        <v>111.777777777778</v>
       </c>
       <c r="D2" s="12">
-        <f>AVERAGE(D10:D14,D16:D20,D21,D23:D28,D30:D36,D38:D43)</f>
-        <v>108.7</v>
+        <f>AVERAGE(D10:D14,D16:D20,D21,D23:D28,D30:D36,D38:D43,D45:D50)</f>
+        <v>109.75</v>
       </c>
       <c r="E2" s="13">
-        <f>AVERAGE(E10:E14,E16:E20,E21,E23:E28,E30:E36,E38:E42)</f>
-        <v>111.689655172414</v>
+        <f>AVERAGE(E10:E14,E16:E20,E21,E23:E28,E30:E36,E38:E42,E45:E50)</f>
+        <v>113.714285714286</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>6</v>
@@ -1245,19 +1249,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="4">
-        <f>MAX(B10:B14,B16:B21,B23:B28,B30:B36,B38:B42)</f>
+        <f>MAX(B10:B14,B16:B21,B23:B28,B30:B36,B38:B42,B45:B50)</f>
         <v>118</v>
       </c>
       <c r="C3" s="4">
-        <f>MAX(C10:C14,C16:C21,C23:C28,C30:C36,C38:C43)</f>
+        <f>MAX(C10:C14,C16:C21,C23:C28,C30:C36,C38:C43,C45:C50)</f>
         <v>161</v>
       </c>
       <c r="D3" s="4">
-        <f>MAX(D10:D14,D16:D21,D23:D28,D30:D36,D38:D43)</f>
-        <v>145</v>
+        <f>MAX(D10:D14,D16:D21,D23:D28,D30:D36,D38:D43,D45:D50)</f>
+        <v>154</v>
       </c>
       <c r="E3" s="6">
-        <f>MAX(E10:E14,E16:E21,E23:E28,E30:E36,E38:E43)</f>
+        <f>MAX(E10:E14,E16:E21,E23:E28,E30:E36,E38:E43,E45:E50)</f>
         <v>180</v>
       </c>
     </row>
@@ -1269,13 +1273,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" s="6">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" s="7" customFormat="1" spans="1:5">
@@ -1291,24 +1295,24 @@
       <c r="D5" s="16">
         <v>1</v>
       </c>
-      <c r="E5" s="17">
-        <v>2</v>
+      <c r="E5" s="18">
+        <v>3</v>
       </c>
     </row>
     <row r="6" s="7" customFormat="1" spans="1:5">
       <c r="A6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="19">
         <v>0</v>
       </c>
-      <c r="C6" s="18">
-        <v>3</v>
-      </c>
-      <c r="D6" s="18">
+      <c r="C6" s="19">
+        <v>4</v>
+      </c>
+      <c r="D6" s="19">
         <v>2</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="19">
         <v>0</v>
       </c>
     </row>
@@ -1316,16 +1320,16 @@
       <c r="A7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="19">
         <v>1</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="19">
         <v>0</v>
       </c>
-      <c r="D7" s="18">
-        <v>2</v>
-      </c>
-      <c r="E7" s="18">
+      <c r="D7" s="19">
+        <v>3</v>
+      </c>
+      <c r="E7" s="19">
         <v>2</v>
       </c>
     </row>
@@ -1333,36 +1337,36 @@
       <c r="A8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="18">
-        <v>4</v>
-      </c>
-      <c r="C8" s="18">
+      <c r="B8" s="19">
+        <v>5</v>
+      </c>
+      <c r="C8" s="19">
         <v>0</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="19">
         <v>0</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="19">
+      <c r="A9" s="20">
         <v>45521</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="21">
         <f>AVERAGE(B10:B14)</f>
         <v>89.8</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="22">
         <f>AVERAGE(C10:C14)</f>
         <v>111.2</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="21">
         <f>AVERAGE(D10:D14)</f>
         <v>99.2</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="21">
         <f>AVERAGE(E10:E14)</f>
         <v>89.2</v>
       </c>
@@ -1371,16 +1375,16 @@
       <c r="A10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="23">
         <v>55</v>
       </c>
       <c r="C10" s="5">
         <v>100</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="23">
         <v>83</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="23">
         <v>83</v>
       </c>
     </row>
@@ -1388,16 +1392,16 @@
       <c r="A11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="23">
         <v>95</v>
       </c>
       <c r="C11" s="5">
         <v>129</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="23">
         <v>92</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="23">
         <v>73</v>
       </c>
     </row>
@@ -1405,16 +1409,16 @@
       <c r="A12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="23">
         <v>100</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="23">
         <v>108</v>
       </c>
       <c r="D12" s="5">
         <v>115</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="23">
         <v>67</v>
       </c>
     </row>
@@ -1422,16 +1426,16 @@
       <c r="A13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="23">
         <v>86</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="23">
         <v>92</v>
       </c>
       <c r="D13" s="5">
         <v>97</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="23">
         <v>95</v>
       </c>
     </row>
@@ -1439,13 +1443,13 @@
       <c r="A14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="23">
         <v>113</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="23">
         <v>127</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="23">
         <v>109</v>
       </c>
       <c r="E14" s="5">
@@ -1453,22 +1457,22 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="19">
+      <c r="A15" s="20">
         <v>45550</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="21">
         <f>AVERAGE(B16:B21)</f>
         <v>91.8333333333333</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="21">
         <f>AVERAGE(C16:C21)</f>
         <v>107.5</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="22">
         <f>AVERAGE(D16:D21)</f>
         <v>123.166666666667</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="21">
         <f>AVERAGE(E16:E21)</f>
         <v>94</v>
       </c>
@@ -1477,13 +1481,13 @@
       <c r="A16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="23">
         <v>118</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="23">
         <v>87</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="23">
         <v>114</v>
       </c>
       <c r="E16" s="5">
@@ -1494,16 +1498,16 @@
       <c r="A17" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="23">
         <v>104</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="23">
         <v>107</v>
       </c>
       <c r="D17" s="5">
         <v>145</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="23">
         <v>93</v>
       </c>
     </row>
@@ -1511,16 +1515,16 @@
       <c r="A18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="23">
         <v>95</v>
       </c>
       <c r="C18" s="5">
         <v>142</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="23">
         <v>132</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="23">
         <v>105</v>
       </c>
     </row>
@@ -1528,16 +1532,16 @@
       <c r="A19" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="23">
         <v>70</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="23">
         <v>99</v>
       </c>
       <c r="D19" s="5">
         <v>102</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="23">
         <v>69</v>
       </c>
     </row>
@@ -1545,16 +1549,16 @@
       <c r="A20" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="23">
         <v>81</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="23">
         <v>108</v>
       </c>
       <c r="D20" s="5">
         <v>122</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="23">
         <v>87</v>
       </c>
     </row>
@@ -1562,36 +1566,36 @@
       <c r="A21" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="23">
         <v>83</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="23">
         <v>102</v>
       </c>
       <c r="D21" s="5">
         <v>124</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="23">
         <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="19">
+      <c r="A22" s="20">
         <v>45557</v>
       </c>
-      <c r="B22" s="20">
+      <c r="B22" s="21">
         <f>AVERAGE(B23:B28)</f>
         <v>106.5</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="22">
         <f>AVERAGE(C23:C28)</f>
         <v>110</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="21">
         <f>AVERAGE(D23:D28)</f>
         <v>109.666666666667</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="21">
         <f>AVERAGE(E23:E28)</f>
         <v>108.5</v>
       </c>
@@ -1600,13 +1604,13 @@
       <c r="A23" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="23">
         <v>85</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="23">
         <v>112</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="23">
         <v>73</v>
       </c>
       <c r="E23" s="5">
@@ -1617,13 +1621,13 @@
       <c r="A24" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="23">
         <v>116</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="23">
         <v>99</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="23">
         <v>93</v>
       </c>
       <c r="E24" s="5">
@@ -1634,16 +1638,16 @@
       <c r="A25" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="23">
         <v>103</v>
       </c>
       <c r="C25" s="5">
         <v>108</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="23">
         <v>104</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="23">
         <v>102</v>
       </c>
     </row>
@@ -1651,16 +1655,16 @@
       <c r="A26" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="22">
+      <c r="B26" s="23">
         <v>103</v>
       </c>
       <c r="C26" s="5">
         <v>147</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="23">
         <v>104</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="23">
         <v>100</v>
       </c>
     </row>
@@ -1668,16 +1672,16 @@
       <c r="A27" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="23">
         <v>115</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="23">
         <v>117</v>
       </c>
       <c r="D27" s="5">
         <v>145</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="23">
         <v>92</v>
       </c>
     </row>
@@ -1685,36 +1689,36 @@
       <c r="A28" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="22">
+      <c r="B28" s="23">
         <v>117</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="23">
         <v>77</v>
       </c>
       <c r="D28" s="5">
         <v>139</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28" s="23">
         <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="19">
+      <c r="A29" s="20">
         <v>45564</v>
       </c>
-      <c r="B29" s="20">
+      <c r="B29" s="21">
         <f>AVERAGE(B30:B36)</f>
         <v>92.2857142857143</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="21">
         <f>AVERAGE(C30:C36)</f>
         <v>117</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="21">
         <f>AVERAGE(D30:D36)</f>
         <v>110.142857142857</v>
       </c>
-      <c r="E29" s="21">
+      <c r="E29" s="22">
         <f>AVERAGE(E30:E36)</f>
         <v>130.857142857143</v>
       </c>
@@ -1723,16 +1727,16 @@
       <c r="A30" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="22">
+      <c r="B30" s="23">
         <v>110</v>
       </c>
-      <c r="C30" s="22">
+      <c r="C30" s="23">
         <v>79</v>
       </c>
       <c r="D30" s="5">
         <v>122</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E30" s="23">
         <v>117</v>
       </c>
     </row>
@@ -1740,13 +1744,13 @@
       <c r="A31" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B31" s="23">
         <v>90</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="23">
         <v>117</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="23">
         <v>125</v>
       </c>
       <c r="E31" s="5">
@@ -1757,16 +1761,16 @@
       <c r="A32" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="22">
+      <c r="B32" s="23">
         <v>75</v>
       </c>
       <c r="C32" s="5">
         <v>161</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32" s="23">
         <v>131</v>
       </c>
-      <c r="E32" s="22">
+      <c r="E32" s="23">
         <v>100</v>
       </c>
     </row>
@@ -1774,13 +1778,13 @@
       <c r="A33" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B33" s="23">
         <v>93</v>
       </c>
-      <c r="C33" s="22">
+      <c r="C33" s="23">
         <v>122</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="23">
         <v>121</v>
       </c>
       <c r="E33" s="5">
@@ -1791,13 +1795,13 @@
       <c r="A34" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="22">
+      <c r="B34" s="23">
         <v>99</v>
       </c>
-      <c r="C34" s="22">
+      <c r="C34" s="23">
         <v>121</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="23">
         <v>71</v>
       </c>
       <c r="E34" s="5">
@@ -1808,13 +1812,13 @@
       <c r="A35" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="22">
+      <c r="B35" s="23">
         <v>82</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="23">
         <v>94</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="23">
         <v>89</v>
       </c>
       <c r="E35" s="5">
@@ -1825,13 +1829,13 @@
       <c r="A36" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="22">
+      <c r="B36" s="23">
         <v>97</v>
       </c>
-      <c r="C36" s="22">
+      <c r="C36" s="23">
         <v>125</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="23">
         <v>112</v>
       </c>
       <c r="E36" s="5">
@@ -1839,22 +1843,22 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="19">
+      <c r="A37" s="20">
         <v>45570</v>
       </c>
-      <c r="B37" s="20">
+      <c r="B37" s="21">
         <f>AVERAGE(B38:B42)</f>
         <v>82.6</v>
       </c>
-      <c r="C37" s="20">
+      <c r="C37" s="21">
         <f>AVERAGE(C38:C43)</f>
         <v>105.333333333333</v>
       </c>
-      <c r="D37" s="20">
+      <c r="D37" s="21">
         <f>AVERAGE(D38:D43)</f>
         <v>99.5</v>
       </c>
-      <c r="E37" s="21">
+      <c r="E37" s="22">
         <f>AVERAGE(E38:E42)</f>
         <v>132.4</v>
       </c>
@@ -1959,6 +1963,129 @@
       </c>
       <c r="E43" s="4" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="20">
+        <v>45577</v>
+      </c>
+      <c r="B44" s="21">
+        <f>AVERAGE(B45:B50)</f>
+        <v>100.833333333333</v>
+      </c>
+      <c r="C44" s="24">
+        <f>AVERAGE(C45:C50)</f>
+        <v>118.666666666667</v>
+      </c>
+      <c r="D44" s="21">
+        <f>AVERAGE(D45:D50)</f>
+        <v>115</v>
+      </c>
+      <c r="E44" s="25">
+        <f>AVERAGE(E45:E50)</f>
+        <v>123.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="23">
+        <v>114</v>
+      </c>
+      <c r="C45" s="23">
+        <v>119</v>
+      </c>
+      <c r="D45" s="5">
+        <v>123</v>
+      </c>
+      <c r="E45" s="26">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="23">
+        <v>107</v>
+      </c>
+      <c r="C46" s="23">
+        <v>121</v>
+      </c>
+      <c r="D46" s="5">
+        <v>154</v>
+      </c>
+      <c r="E46" s="26">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="23">
+        <v>75</v>
+      </c>
+      <c r="C47" s="26">
+        <v>94</v>
+      </c>
+      <c r="D47" s="23">
+        <v>107</v>
+      </c>
+      <c r="E47" s="5">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="23">
+        <v>109</v>
+      </c>
+      <c r="C48" s="5">
+        <v>145</v>
+      </c>
+      <c r="D48" s="23">
+        <v>119</v>
+      </c>
+      <c r="E48" s="23">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" s="23">
+        <v>107</v>
+      </c>
+      <c r="C49" s="23">
+        <v>115</v>
+      </c>
+      <c r="D49" s="26">
+        <v>102</v>
+      </c>
+      <c r="E49" s="5">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="23">
+        <v>93</v>
+      </c>
+      <c r="C50" s="23">
+        <v>118</v>
+      </c>
+      <c r="D50" s="26">
+        <v>85</v>
+      </c>
+      <c r="E50" s="5">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1972,8 +2099,8 @@
   <sheetPr/>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -2021,26 +2148,26 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
       <c r="D2" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
       </c>
       <c r="F2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H2" s="2">
         <f>SUM(4*C2,3*D2,2*E2,1*F2,G2)</f>
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" ht="25" customHeight="1" spans="1:8">
@@ -2048,26 +2175,26 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="2">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
       <c r="G3" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H3" s="2">
         <f>SUM(4*C3,3*D3,2*E3,1*F3,G3)</f>
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:8">
@@ -2081,7 +2208,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -2090,11 +2217,11 @@
         <v>0</v>
       </c>
       <c r="G4" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H4" s="2">
         <f>SUM(4*C4,3*D4,2*E4,1*F4,G4)</f>
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" ht="27" customHeight="1" spans="1:8">
@@ -2114,14 +2241,14 @@
         <v>1</v>
       </c>
       <c r="F5" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
       </c>
       <c r="H5" s="2">
         <f>SUM(4*C5,3*D5,2*E5,1*F5,G5)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2181,7 +2308,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I5">
+  <sortState ref="A2:H14">
     <sortCondition ref="H2" descending="1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
19 Oct results update
</commit_message>
<xml_diff>
--- a/public/bowling_weekly_scores.xlsx
+++ b/public/bowling_weekly_scores.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
   <si>
     <t>Bowler</t>
   </si>
@@ -153,7 +153,7 @@
     <numFmt numFmtId="180" formatCode="0.00_ "/>
     <numFmt numFmtId="181" formatCode="0_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +178,13 @@
     <font>
       <sz val="11"/>
       <color theme="9"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.25"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -690,133 +697,133 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -850,7 +857,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="181" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="181" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -860,7 +866,8 @@
     <xf numFmtId="180" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="180" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1186,12 +1193,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1225,20 +1232,20 @@
         <v>5</v>
       </c>
       <c r="B2" s="12">
-        <f>AVERAGE(B10:B14,B16:B20,B21,B23:B28,B30:B36,B38:B42,B45:B50)</f>
-        <v>94.3714285714286</v>
-      </c>
-      <c r="C2" s="12">
-        <f>AVERAGE(C10:C14,C16:C20,C21,C23:C28,C30:C36,C38:C43,C45:C50)</f>
-        <v>111.777777777778</v>
+        <f>AVERAGE(B10:B14,B16:B20,B21,B23:B28,B30:B36,B38:B42,B45:B50,B52:B57)</f>
+        <v>96.3170731707317</v>
+      </c>
+      <c r="C2" s="13">
+        <f>AVERAGE(C10:C14,C16:C20,C21,C23:C28,C30:C36,C38:C42,C45:C50,C52:C57)</f>
+        <v>115.878048780488</v>
       </c>
       <c r="D2" s="12">
-        <f>AVERAGE(D10:D14,D16:D20,D21,D23:D28,D30:D36,D38:D43,D45:D50)</f>
-        <v>109.75</v>
-      </c>
-      <c r="E2" s="13">
-        <f>AVERAGE(E10:E14,E16:E20,E21,E23:E28,E30:E36,E38:E42,E45:E50)</f>
-        <v>113.714285714286</v>
+        <f>AVERAGE(D10:D14,D16:D20,D21,D23:D28,D30:D36,D38:D42,D45:D50,D52:D57)</f>
+        <v>110.268292682927</v>
+      </c>
+      <c r="E2" s="12">
+        <f>AVERAGE(E10:E14,E16:E20,E21,E23:E28,E30:E36,E38:E42,E45:E50,E52:E57)</f>
+        <v>113.024390243902</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>6</v>
@@ -1249,19 +1256,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="4">
-        <f>MAX(B10:B14,B16:B21,B23:B28,B30:B36,B38:B42,B45:B50)</f>
-        <v>118</v>
+        <f>MAX(B10:B14,B16:B21,B23:B28,B30:B36,B38:B42,B45:B50,B52:B57)</f>
+        <v>136</v>
       </c>
       <c r="C3" s="4">
-        <f>MAX(C10:C14,C16:C21,C23:C28,C30:C36,C38:C43,C45:C50)</f>
+        <f>MAX(C10:C14,C16:C21,C23:C28,C30:C36,C38:C42,C45:C50,C52:C57)</f>
         <v>161</v>
       </c>
       <c r="D3" s="4">
-        <f>MAX(D10:D14,D16:D21,D23:D28,D30:D36,D38:D43,D45:D50)</f>
+        <f>MAX(D10:D14,D16:D21,D23:D28,D30:D36,D38:D42,D45:D50,D52:D57)</f>
         <v>154</v>
       </c>
       <c r="E3" s="6">
-        <f>MAX(E10:E14,E16:E21,E23:E28,E30:E36,E38:E43,E45:E50)</f>
+        <f>MAX(E10:E14,E16:E21,E23:E28,E30:E36,E38:E42,E45:E50,E52:E57)</f>
         <v>180</v>
       </c>
     </row>
@@ -1270,13 +1277,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D4" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="6">
         <v>15</v>
@@ -1290,12 +1297,12 @@
         <v>0</v>
       </c>
       <c r="C5" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="16">
         <v>1</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <v>3</v>
       </c>
     </row>
@@ -1303,16 +1310,16 @@
       <c r="A6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="18">
         <v>0</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="18">
         <v>4</v>
       </c>
-      <c r="D6" s="19">
-        <v>2</v>
-      </c>
-      <c r="E6" s="19">
+      <c r="D6" s="18">
+        <v>3</v>
+      </c>
+      <c r="E6" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1320,53 +1327,53 @@
       <c r="A7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="18">
         <v>1</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="18">
         <v>0</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="18">
         <v>3</v>
       </c>
-      <c r="E7" s="19">
-        <v>2</v>
+      <c r="E7" s="18">
+        <v>3</v>
       </c>
     </row>
     <row r="8" s="7" customFormat="1" spans="1:5">
       <c r="A8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="19">
-        <v>5</v>
-      </c>
-      <c r="C8" s="19">
+      <c r="B8" s="18">
+        <v>6</v>
+      </c>
+      <c r="C8" s="18">
         <v>0</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="18">
         <v>0</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="20">
+      <c r="A9" s="19">
         <v>45521</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="20">
         <f>AVERAGE(B10:B14)</f>
         <v>89.8</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="21">
         <f>AVERAGE(C10:C14)</f>
         <v>111.2</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <f>AVERAGE(D10:D14)</f>
         <v>99.2</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="20">
         <f>AVERAGE(E10:E14)</f>
         <v>89.2</v>
       </c>
@@ -1375,16 +1382,16 @@
       <c r="A10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="22">
         <v>55</v>
       </c>
       <c r="C10" s="5">
         <v>100</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="22">
         <v>83</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="22">
         <v>83</v>
       </c>
     </row>
@@ -1392,16 +1399,16 @@
       <c r="A11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="22">
         <v>95</v>
       </c>
       <c r="C11" s="5">
         <v>129</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="22">
         <v>92</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="22">
         <v>73</v>
       </c>
     </row>
@@ -1409,16 +1416,16 @@
       <c r="A12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="22">
         <v>100</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="22">
         <v>108</v>
       </c>
       <c r="D12" s="5">
         <v>115</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="22">
         <v>67</v>
       </c>
     </row>
@@ -1426,16 +1433,16 @@
       <c r="A13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="22">
         <v>86</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="22">
         <v>92</v>
       </c>
       <c r="D13" s="5">
         <v>97</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="22">
         <v>95</v>
       </c>
     </row>
@@ -1443,13 +1450,13 @@
       <c r="A14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="22">
         <v>113</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="22">
         <v>127</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="22">
         <v>109</v>
       </c>
       <c r="E14" s="5">
@@ -1457,22 +1464,22 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="20">
+      <c r="A15" s="19">
         <v>45550</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="20">
         <f>AVERAGE(B16:B21)</f>
         <v>91.8333333333333</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="20">
         <f>AVERAGE(C16:C21)</f>
         <v>107.5</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="21">
         <f>AVERAGE(D16:D21)</f>
         <v>123.166666666667</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="20">
         <f>AVERAGE(E16:E21)</f>
         <v>94</v>
       </c>
@@ -1481,13 +1488,13 @@
       <c r="A16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="22">
         <v>118</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="22">
         <v>87</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="22">
         <v>114</v>
       </c>
       <c r="E16" s="5">
@@ -1498,16 +1505,16 @@
       <c r="A17" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="22">
         <v>104</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="22">
         <v>107</v>
       </c>
       <c r="D17" s="5">
         <v>145</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="22">
         <v>93</v>
       </c>
     </row>
@@ -1515,16 +1522,16 @@
       <c r="A18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="22">
         <v>95</v>
       </c>
       <c r="C18" s="5">
         <v>142</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="22">
         <v>132</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="22">
         <v>105</v>
       </c>
     </row>
@@ -1532,16 +1539,16 @@
       <c r="A19" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B19" s="22">
         <v>70</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="22">
         <v>99</v>
       </c>
       <c r="D19" s="5">
         <v>102</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="22">
         <v>69</v>
       </c>
     </row>
@@ -1549,16 +1556,16 @@
       <c r="A20" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="22">
         <v>81</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="22">
         <v>108</v>
       </c>
       <c r="D20" s="5">
         <v>122</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="22">
         <v>87</v>
       </c>
     </row>
@@ -1566,36 +1573,36 @@
       <c r="A21" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B21" s="22">
         <v>83</v>
       </c>
-      <c r="C21" s="23">
+      <c r="C21" s="22">
         <v>102</v>
       </c>
       <c r="D21" s="5">
         <v>124</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="22">
         <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="20">
+      <c r="A22" s="19">
         <v>45557</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="20">
         <f>AVERAGE(B23:B28)</f>
         <v>106.5</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="21">
         <f>AVERAGE(C23:C28)</f>
         <v>110</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="20">
         <f>AVERAGE(D23:D28)</f>
         <v>109.666666666667</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="20">
         <f>AVERAGE(E23:E28)</f>
         <v>108.5</v>
       </c>
@@ -1604,13 +1611,13 @@
       <c r="A23" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="22">
         <v>85</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C23" s="22">
         <v>112</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="22">
         <v>73</v>
       </c>
       <c r="E23" s="5">
@@ -1621,13 +1628,13 @@
       <c r="A24" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="22">
         <v>116</v>
       </c>
-      <c r="C24" s="23">
+      <c r="C24" s="22">
         <v>99</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="22">
         <v>93</v>
       </c>
       <c r="E24" s="5">
@@ -1638,16 +1645,16 @@
       <c r="A25" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B25" s="22">
         <v>103</v>
       </c>
       <c r="C25" s="5">
         <v>108</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="22">
         <v>104</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="22">
         <v>102</v>
       </c>
     </row>
@@ -1655,16 +1662,16 @@
       <c r="A26" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B26" s="22">
         <v>103</v>
       </c>
       <c r="C26" s="5">
         <v>147</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="22">
         <v>104</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="22">
         <v>100</v>
       </c>
     </row>
@@ -1672,16 +1679,16 @@
       <c r="A27" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="23">
+      <c r="B27" s="22">
         <v>115</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C27" s="22">
         <v>117</v>
       </c>
       <c r="D27" s="5">
         <v>145</v>
       </c>
-      <c r="E27" s="23">
+      <c r="E27" s="22">
         <v>92</v>
       </c>
     </row>
@@ -1689,36 +1696,36 @@
       <c r="A28" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="23">
+      <c r="B28" s="22">
         <v>117</v>
       </c>
-      <c r="C28" s="23">
+      <c r="C28" s="22">
         <v>77</v>
       </c>
       <c r="D28" s="5">
         <v>139</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="22">
         <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="20">
+      <c r="A29" s="19">
         <v>45564</v>
       </c>
-      <c r="B29" s="21">
+      <c r="B29" s="20">
         <f>AVERAGE(B30:B36)</f>
         <v>92.2857142857143</v>
       </c>
-      <c r="C29" s="21">
+      <c r="C29" s="20">
         <f>AVERAGE(C30:C36)</f>
         <v>117</v>
       </c>
-      <c r="D29" s="21">
+      <c r="D29" s="20">
         <f>AVERAGE(D30:D36)</f>
         <v>110.142857142857</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="21">
         <f>AVERAGE(E30:E36)</f>
         <v>130.857142857143</v>
       </c>
@@ -1727,16 +1734,16 @@
       <c r="A30" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="23">
+      <c r="B30" s="22">
         <v>110</v>
       </c>
-      <c r="C30" s="23">
+      <c r="C30" s="22">
         <v>79</v>
       </c>
       <c r="D30" s="5">
         <v>122</v>
       </c>
-      <c r="E30" s="23">
+      <c r="E30" s="22">
         <v>117</v>
       </c>
     </row>
@@ -1744,13 +1751,13 @@
       <c r="A31" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="23">
+      <c r="B31" s="22">
         <v>90</v>
       </c>
-      <c r="C31" s="23">
+      <c r="C31" s="22">
         <v>117</v>
       </c>
-      <c r="D31" s="23">
+      <c r="D31" s="22">
         <v>125</v>
       </c>
       <c r="E31" s="5">
@@ -1761,16 +1768,16 @@
       <c r="A32" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="23">
+      <c r="B32" s="22">
         <v>75</v>
       </c>
       <c r="C32" s="5">
         <v>161</v>
       </c>
-      <c r="D32" s="23">
+      <c r="D32" s="22">
         <v>131</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="22">
         <v>100</v>
       </c>
     </row>
@@ -1778,13 +1785,13 @@
       <c r="A33" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="23">
+      <c r="B33" s="22">
         <v>93</v>
       </c>
-      <c r="C33" s="23">
+      <c r="C33" s="22">
         <v>122</v>
       </c>
-      <c r="D33" s="23">
+      <c r="D33" s="22">
         <v>121</v>
       </c>
       <c r="E33" s="5">
@@ -1795,13 +1802,13 @@
       <c r="A34" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="23">
+      <c r="B34" s="22">
         <v>99</v>
       </c>
-      <c r="C34" s="23">
+      <c r="C34" s="22">
         <v>121</v>
       </c>
-      <c r="D34" s="23">
+      <c r="D34" s="22">
         <v>71</v>
       </c>
       <c r="E34" s="5">
@@ -1812,13 +1819,13 @@
       <c r="A35" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="23">
+      <c r="B35" s="22">
         <v>82</v>
       </c>
-      <c r="C35" s="23">
+      <c r="C35" s="22">
         <v>94</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="22">
         <v>89</v>
       </c>
       <c r="E35" s="5">
@@ -1829,13 +1836,13 @@
       <c r="A36" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="23">
+      <c r="B36" s="22">
         <v>97</v>
       </c>
-      <c r="C36" s="23">
+      <c r="C36" s="22">
         <v>125</v>
       </c>
-      <c r="D36" s="23">
+      <c r="D36" s="22">
         <v>112</v>
       </c>
       <c r="E36" s="5">
@@ -1843,22 +1850,22 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="20">
+      <c r="A37" s="19">
         <v>45570</v>
       </c>
-      <c r="B37" s="21">
+      <c r="B37" s="20">
         <f>AVERAGE(B38:B42)</f>
         <v>82.6</v>
       </c>
-      <c r="C37" s="21">
+      <c r="C37" s="20">
         <f>AVERAGE(C38:C43)</f>
         <v>105.333333333333</v>
       </c>
-      <c r="D37" s="21">
+      <c r="D37" s="20">
         <f>AVERAGE(D38:D43)</f>
         <v>99.5</v>
       </c>
-      <c r="E37" s="22">
+      <c r="E37" s="21">
         <f>AVERAGE(E38:E42)</f>
         <v>132.4</v>
       </c>
@@ -1966,22 +1973,22 @@
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="20">
+      <c r="A44" s="19">
         <v>45577</v>
       </c>
-      <c r="B44" s="21">
+      <c r="B44" s="20">
         <f>AVERAGE(B45:B50)</f>
         <v>100.833333333333</v>
       </c>
-      <c r="C44" s="24">
+      <c r="C44" s="23">
         <f>AVERAGE(C45:C50)</f>
         <v>118.666666666667</v>
       </c>
-      <c r="D44" s="21">
+      <c r="D44" s="20">
         <f>AVERAGE(D45:D50)</f>
         <v>115</v>
       </c>
-      <c r="E44" s="25">
+      <c r="E44" s="21">
         <f>AVERAGE(E45:E50)</f>
         <v>123.5</v>
       </c>
@@ -1990,16 +1997,16 @@
       <c r="A45" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="23">
+      <c r="B45" s="22">
         <v>114</v>
       </c>
-      <c r="C45" s="23">
+      <c r="C45" s="22">
         <v>119</v>
       </c>
       <c r="D45" s="5">
         <v>123</v>
       </c>
-      <c r="E45" s="26">
+      <c r="E45" s="22">
         <v>103</v>
       </c>
     </row>
@@ -2007,16 +2014,16 @@
       <c r="A46" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="23">
+      <c r="B46" s="22">
         <v>107</v>
       </c>
-      <c r="C46" s="23">
+      <c r="C46" s="22">
         <v>121</v>
       </c>
       <c r="D46" s="5">
         <v>154</v>
       </c>
-      <c r="E46" s="26">
+      <c r="E46" s="22">
         <v>77</v>
       </c>
     </row>
@@ -2024,13 +2031,13 @@
       <c r="A47" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="23">
+      <c r="B47" s="22">
         <v>75</v>
       </c>
-      <c r="C47" s="26">
+      <c r="C47" s="22">
         <v>94</v>
       </c>
-      <c r="D47" s="23">
+      <c r="D47" s="22">
         <v>107</v>
       </c>
       <c r="E47" s="5">
@@ -2041,16 +2048,16 @@
       <c r="A48" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="23">
+      <c r="B48" s="22">
         <v>109</v>
       </c>
       <c r="C48" s="5">
         <v>145</v>
       </c>
-      <c r="D48" s="23">
+      <c r="D48" s="22">
         <v>119</v>
       </c>
-      <c r="E48" s="23">
+      <c r="E48" s="22">
         <v>126</v>
       </c>
     </row>
@@ -2058,13 +2065,13 @@
       <c r="A49" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="23">
+      <c r="B49" s="22">
         <v>107</v>
       </c>
-      <c r="C49" s="23">
+      <c r="C49" s="22">
         <v>115</v>
       </c>
-      <c r="D49" s="26">
+      <c r="D49" s="22">
         <v>102</v>
       </c>
       <c r="E49" s="5">
@@ -2075,17 +2082,140 @@
       <c r="A50" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="23">
+      <c r="B50" s="22">
         <v>93</v>
       </c>
-      <c r="C50" s="23">
+      <c r="C50" s="22">
         <v>118</v>
       </c>
-      <c r="D50" s="26">
+      <c r="D50" s="22">
         <v>85</v>
       </c>
       <c r="E50" s="5">
         <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="19">
+        <v>45577</v>
+      </c>
+      <c r="B51" s="20">
+        <f>AVERAGE(B52:B57)</f>
+        <v>107.666666666667</v>
+      </c>
+      <c r="C51" s="24">
+        <f>AVERAGE(C52:C57)</f>
+        <v>139.166666666667</v>
+      </c>
+      <c r="D51" s="20">
+        <f>AVERAGE(D52:D57)</f>
+        <v>111.5</v>
+      </c>
+      <c r="E51" s="23">
+        <f>AVERAGE(E52:E57)</f>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="25">
+        <v>106</v>
+      </c>
+      <c r="C52" s="5">
+        <v>157</v>
+      </c>
+      <c r="D52" s="26">
+        <v>102</v>
+      </c>
+      <c r="E52" s="25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="25">
+        <v>136</v>
+      </c>
+      <c r="C53" s="5">
+        <v>144</v>
+      </c>
+      <c r="D53" s="26">
+        <v>97</v>
+      </c>
+      <c r="E53" s="25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" s="25">
+        <v>96</v>
+      </c>
+      <c r="C54" s="25">
+        <v>122</v>
+      </c>
+      <c r="D54" s="5">
+        <v>136</v>
+      </c>
+      <c r="E54" s="26">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="25">
+        <v>83</v>
+      </c>
+      <c r="C55" s="5">
+        <v>141</v>
+      </c>
+      <c r="D55" s="25">
+        <v>88</v>
+      </c>
+      <c r="E55" s="25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="5">
+        <v>133</v>
+      </c>
+      <c r="C56" s="25">
+        <v>111</v>
+      </c>
+      <c r="D56" s="25">
+        <v>108</v>
+      </c>
+      <c r="E56" s="26">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="25">
+        <v>92</v>
+      </c>
+      <c r="C57" s="5">
+        <v>160</v>
+      </c>
+      <c r="D57" s="25">
+        <v>138</v>
+      </c>
+      <c r="E57" s="26">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2100,7 +2230,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -2148,26 +2278,26 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
       </c>
       <c r="D2" s="2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
-        <v>2</v>
-      </c>
       <c r="F2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2">
         <f>SUM(4*C2,3*D2,2*E2,1*F2,G2)</f>
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" ht="25" customHeight="1" spans="1:8">
@@ -2175,26 +2305,26 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
         <v>3</v>
       </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
       <c r="D3" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2">
         <v>3</v>
       </c>
       <c r="F3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H3" s="2">
         <f>SUM(4*C3,3*D3,2*E3,1*F3,G3)</f>
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:8">
@@ -2202,26 +2332,26 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="2">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H4" s="2">
         <f>SUM(4*C4,3*D4,2*E4,1*F4,G4)</f>
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" ht="27" customHeight="1" spans="1:8">
@@ -2241,14 +2371,14 @@
         <v>1</v>
       </c>
       <c r="F5" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="2">
         <f>SUM(4*C5,3*D5,2*E5,1*F5,G5)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2">

</xml_diff>

<commit_message>
11 Jan results update
</commit_message>
<xml_diff>
--- a/public/bowling_weekly_scores.xlsx
+++ b/public/bowling_weekly_scores.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>Bowler</t>
   </si>
@@ -827,7 +827,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -858,6 +858,7 @@
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="181" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="181" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1193,12 +1194,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H60" sqref="H60"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1232,20 +1233,20 @@
         <v>5</v>
       </c>
       <c r="B2" s="12">
-        <f>AVERAGE(B10:B14,B16:B20,B21,B23:B28,B30:B36,B38:B42,B45:B50,B52:B57)</f>
-        <v>96.3170731707317</v>
+        <f>AVERAGE(B10:B14,B16:B20,B21,B23:B28,B30:B36,B38:B42,B45:B50,B52:B57,B59:B63)</f>
+        <v>98.1304347826087</v>
       </c>
       <c r="C2" s="13">
-        <f>AVERAGE(C10:C14,C16:C20,C21,C23:C28,C30:C36,C38:C42,C45:C50,C52:C57)</f>
-        <v>115.878048780488</v>
+        <f>AVERAGE(C10:C14,C16:C20,C21,C23:C28,C30:C36,C38:C42,C45:C50,C52:C57,C59:C63)</f>
+        <v>116.652173913043</v>
       </c>
       <c r="D2" s="12">
-        <f>AVERAGE(D10:D14,D16:D20,D21,D23:D28,D30:D36,D38:D42,D45:D50,D52:D57)</f>
-        <v>110.268292682927</v>
+        <f>AVERAGE(D10:D14,D16:D20,D21,D23:D28,D30:D36,D38:D42,D45:D50,D52:D57,D59:D63)</f>
+        <v>109.760869565217</v>
       </c>
       <c r="E2" s="12">
-        <f>AVERAGE(E10:E14,E16:E20,E21,E23:E28,E30:E36,E38:E42,E45:E50,E52:E57)</f>
-        <v>113.024390243902</v>
+        <f>AVERAGE(E10:E14,E16:E20,E21,E23:E28,E30:E36,E38:E42,E45:E50,E52:E57,E59:E63)</f>
+        <v>111.717391304348</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>6</v>
@@ -1256,19 +1257,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="4">
-        <f>MAX(B10:B14,B16:B21,B23:B28,B30:B36,B38:B42,B45:B50,B52:B57)</f>
-        <v>136</v>
+        <f>MAX(B10:B14,B16:B21,B23:B28,B30:B36,B38:B42,B45:B50,B52:B57,B59:B63)</f>
+        <v>146</v>
       </c>
       <c r="C3" s="4">
-        <f>MAX(C10:C14,C16:C21,C23:C28,C30:C36,C38:C42,C45:C50,C52:C57)</f>
+        <f>MAX(C10:C14,C16:C21,C23:C28,C30:C36,C38:C42,C45:C50,C52:C57,C59:C63)</f>
         <v>161</v>
       </c>
       <c r="D3" s="4">
-        <f>MAX(D10:D14,D16:D21,D23:D28,D30:D36,D38:D42,D45:D50,D52:D57)</f>
+        <f>MAX(D10:D14,D16:D21,D23:D28,D30:D36,D38:D42,D45:D50,D52:D57,D59:D63)</f>
         <v>154</v>
       </c>
       <c r="E3" s="6">
-        <f>MAX(E10:E14,E16:E21,E23:E28,E30:E36,E38:E42,E45:E50,E52:E57)</f>
+        <f>MAX(E10:E14,E16:E21,E23:E28,E30:E36,E38:E42,E45:E50,E52:E57,E59:E63)</f>
         <v>180</v>
       </c>
     </row>
@@ -1277,16 +1278,16 @@
         <v>8</v>
       </c>
       <c r="B4" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4">
         <v>14</v>
       </c>
       <c r="E4" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" s="7" customFormat="1" spans="1:5">
@@ -1297,12 +1298,12 @@
         <v>0</v>
       </c>
       <c r="C5" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="16">
         <v>1</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="18">
         <v>3</v>
       </c>
     </row>
@@ -1310,16 +1311,16 @@
       <c r="A6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="18">
-        <v>0</v>
-      </c>
-      <c r="C6" s="18">
+      <c r="B6" s="19">
+        <v>1</v>
+      </c>
+      <c r="C6" s="19">
         <v>4</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="19">
         <v>3</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="19">
         <v>0</v>
       </c>
     </row>
@@ -1327,16 +1328,16 @@
       <c r="A7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="19">
         <v>1</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="19">
         <v>0</v>
       </c>
-      <c r="D7" s="18">
-        <v>3</v>
-      </c>
-      <c r="E7" s="18">
+      <c r="D7" s="19">
+        <v>4</v>
+      </c>
+      <c r="E7" s="19">
         <v>3</v>
       </c>
     </row>
@@ -1344,36 +1345,36 @@
       <c r="A8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="19">
         <v>6</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="19">
         <v>0</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="19">
         <v>0</v>
       </c>
-      <c r="E8" s="18">
-        <v>1</v>
+      <c r="E8" s="19">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="19">
+      <c r="A9" s="20">
         <v>45521</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="21">
         <f>AVERAGE(B10:B14)</f>
         <v>89.8</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="22">
         <f>AVERAGE(C10:C14)</f>
         <v>111.2</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="21">
         <f>AVERAGE(D10:D14)</f>
         <v>99.2</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="21">
         <f>AVERAGE(E10:E14)</f>
         <v>89.2</v>
       </c>
@@ -1382,16 +1383,16 @@
       <c r="A10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="23">
         <v>55</v>
       </c>
       <c r="C10" s="5">
         <v>100</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="23">
         <v>83</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="23">
         <v>83</v>
       </c>
     </row>
@@ -1399,16 +1400,16 @@
       <c r="A11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="23">
         <v>95</v>
       </c>
       <c r="C11" s="5">
         <v>129</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="23">
         <v>92</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="23">
         <v>73</v>
       </c>
     </row>
@@ -1416,16 +1417,16 @@
       <c r="A12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="23">
         <v>100</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="23">
         <v>108</v>
       </c>
       <c r="D12" s="5">
         <v>115</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="23">
         <v>67</v>
       </c>
     </row>
@@ -1433,16 +1434,16 @@
       <c r="A13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="23">
         <v>86</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="23">
         <v>92</v>
       </c>
       <c r="D13" s="5">
         <v>97</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="23">
         <v>95</v>
       </c>
     </row>
@@ -1450,13 +1451,13 @@
       <c r="A14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="23">
         <v>113</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="23">
         <v>127</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="23">
         <v>109</v>
       </c>
       <c r="E14" s="5">
@@ -1464,22 +1465,22 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="19">
+      <c r="A15" s="20">
         <v>45550</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="21">
         <f>AVERAGE(B16:B21)</f>
         <v>91.8333333333333</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="21">
         <f>AVERAGE(C16:C21)</f>
         <v>107.5</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="22">
         <f>AVERAGE(D16:D21)</f>
         <v>123.166666666667</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="21">
         <f>AVERAGE(E16:E21)</f>
         <v>94</v>
       </c>
@@ -1488,13 +1489,13 @@
       <c r="A16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="23">
         <v>118</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="23">
         <v>87</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="23">
         <v>114</v>
       </c>
       <c r="E16" s="5">
@@ -1505,16 +1506,16 @@
       <c r="A17" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="23">
         <v>104</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="23">
         <v>107</v>
       </c>
       <c r="D17" s="5">
         <v>145</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="23">
         <v>93</v>
       </c>
     </row>
@@ -1522,16 +1523,16 @@
       <c r="A18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="23">
         <v>95</v>
       </c>
       <c r="C18" s="5">
         <v>142</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="23">
         <v>132</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="23">
         <v>105</v>
       </c>
     </row>
@@ -1539,16 +1540,16 @@
       <c r="A19" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="23">
         <v>70</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="23">
         <v>99</v>
       </c>
       <c r="D19" s="5">
         <v>102</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="23">
         <v>69</v>
       </c>
     </row>
@@ -1556,16 +1557,16 @@
       <c r="A20" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="23">
         <v>81</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="23">
         <v>108</v>
       </c>
       <c r="D20" s="5">
         <v>122</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="23">
         <v>87</v>
       </c>
     </row>
@@ -1573,36 +1574,36 @@
       <c r="A21" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="23">
         <v>83</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="23">
         <v>102</v>
       </c>
       <c r="D21" s="5">
         <v>124</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="23">
         <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="19">
+      <c r="A22" s="20">
         <v>45557</v>
       </c>
-      <c r="B22" s="20">
+      <c r="B22" s="21">
         <f>AVERAGE(B23:B28)</f>
         <v>106.5</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="22">
         <f>AVERAGE(C23:C28)</f>
         <v>110</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="21">
         <f>AVERAGE(D23:D28)</f>
         <v>109.666666666667</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="21">
         <f>AVERAGE(E23:E28)</f>
         <v>108.5</v>
       </c>
@@ -1611,13 +1612,13 @@
       <c r="A23" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="23">
         <v>85</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="23">
         <v>112</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="23">
         <v>73</v>
       </c>
       <c r="E23" s="5">
@@ -1628,13 +1629,13 @@
       <c r="A24" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="23">
         <v>116</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="23">
         <v>99</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="23">
         <v>93</v>
       </c>
       <c r="E24" s="5">
@@ -1645,16 +1646,16 @@
       <c r="A25" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="23">
         <v>103</v>
       </c>
       <c r="C25" s="5">
         <v>108</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="23">
         <v>104</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="23">
         <v>102</v>
       </c>
     </row>
@@ -1662,16 +1663,16 @@
       <c r="A26" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="22">
+      <c r="B26" s="23">
         <v>103</v>
       </c>
       <c r="C26" s="5">
         <v>147</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="23">
         <v>104</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="23">
         <v>100</v>
       </c>
     </row>
@@ -1679,16 +1680,16 @@
       <c r="A27" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="23">
         <v>115</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="23">
         <v>117</v>
       </c>
       <c r="D27" s="5">
         <v>145</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="23">
         <v>92</v>
       </c>
     </row>
@@ -1696,36 +1697,36 @@
       <c r="A28" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="22">
+      <c r="B28" s="23">
         <v>117</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="23">
         <v>77</v>
       </c>
       <c r="D28" s="5">
         <v>139</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28" s="23">
         <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="19">
+      <c r="A29" s="20">
         <v>45564</v>
       </c>
-      <c r="B29" s="20">
+      <c r="B29" s="21">
         <f>AVERAGE(B30:B36)</f>
         <v>92.2857142857143</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="21">
         <f>AVERAGE(C30:C36)</f>
         <v>117</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="21">
         <f>AVERAGE(D30:D36)</f>
         <v>110.142857142857</v>
       </c>
-      <c r="E29" s="21">
+      <c r="E29" s="22">
         <f>AVERAGE(E30:E36)</f>
         <v>130.857142857143</v>
       </c>
@@ -1734,16 +1735,16 @@
       <c r="A30" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="22">
+      <c r="B30" s="23">
         <v>110</v>
       </c>
-      <c r="C30" s="22">
+      <c r="C30" s="23">
         <v>79</v>
       </c>
       <c r="D30" s="5">
         <v>122</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E30" s="23">
         <v>117</v>
       </c>
     </row>
@@ -1751,13 +1752,13 @@
       <c r="A31" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B31" s="23">
         <v>90</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="23">
         <v>117</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="23">
         <v>125</v>
       </c>
       <c r="E31" s="5">
@@ -1768,16 +1769,16 @@
       <c r="A32" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="22">
+      <c r="B32" s="23">
         <v>75</v>
       </c>
       <c r="C32" s="5">
         <v>161</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32" s="23">
         <v>131</v>
       </c>
-      <c r="E32" s="22">
+      <c r="E32" s="23">
         <v>100</v>
       </c>
     </row>
@@ -1785,13 +1786,13 @@
       <c r="A33" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B33" s="23">
         <v>93</v>
       </c>
-      <c r="C33" s="22">
+      <c r="C33" s="23">
         <v>122</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="23">
         <v>121</v>
       </c>
       <c r="E33" s="5">
@@ -1802,13 +1803,13 @@
       <c r="A34" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="22">
+      <c r="B34" s="23">
         <v>99</v>
       </c>
-      <c r="C34" s="22">
+      <c r="C34" s="23">
         <v>121</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="23">
         <v>71</v>
       </c>
       <c r="E34" s="5">
@@ -1819,13 +1820,13 @@
       <c r="A35" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="22">
+      <c r="B35" s="23">
         <v>82</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="23">
         <v>94</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="23">
         <v>89</v>
       </c>
       <c r="E35" s="5">
@@ -1836,13 +1837,13 @@
       <c r="A36" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="22">
+      <c r="B36" s="23">
         <v>97</v>
       </c>
-      <c r="C36" s="22">
+      <c r="C36" s="23">
         <v>125</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="23">
         <v>112</v>
       </c>
       <c r="E36" s="5">
@@ -1850,22 +1851,22 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="19">
+      <c r="A37" s="20">
         <v>45570</v>
       </c>
-      <c r="B37" s="20">
+      <c r="B37" s="21">
         <f>AVERAGE(B38:B42)</f>
         <v>82.6</v>
       </c>
-      <c r="C37" s="20">
+      <c r="C37" s="21">
         <f>AVERAGE(C38:C43)</f>
         <v>105.333333333333</v>
       </c>
-      <c r="D37" s="20">
+      <c r="D37" s="21">
         <f>AVERAGE(D38:D43)</f>
         <v>99.5</v>
       </c>
-      <c r="E37" s="21">
+      <c r="E37" s="22">
         <f>AVERAGE(E38:E42)</f>
         <v>132.4</v>
       </c>
@@ -1973,22 +1974,22 @@
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="19">
+      <c r="A44" s="20">
         <v>45577</v>
       </c>
-      <c r="B44" s="20">
+      <c r="B44" s="21">
         <f>AVERAGE(B45:B50)</f>
         <v>100.833333333333</v>
       </c>
-      <c r="C44" s="23">
+      <c r="C44" s="24">
         <f>AVERAGE(C45:C50)</f>
         <v>118.666666666667</v>
       </c>
-      <c r="D44" s="20">
+      <c r="D44" s="21">
         <f>AVERAGE(D45:D50)</f>
         <v>115</v>
       </c>
-      <c r="E44" s="21">
+      <c r="E44" s="22">
         <f>AVERAGE(E45:E50)</f>
         <v>123.5</v>
       </c>
@@ -1997,16 +1998,16 @@
       <c r="A45" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22">
+      <c r="B45" s="23">
         <v>114</v>
       </c>
-      <c r="C45" s="22">
+      <c r="C45" s="23">
         <v>119</v>
       </c>
       <c r="D45" s="5">
         <v>123</v>
       </c>
-      <c r="E45" s="22">
+      <c r="E45" s="23">
         <v>103</v>
       </c>
     </row>
@@ -2014,16 +2015,16 @@
       <c r="A46" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="22">
+      <c r="B46" s="23">
         <v>107</v>
       </c>
-      <c r="C46" s="22">
+      <c r="C46" s="23">
         <v>121</v>
       </c>
       <c r="D46" s="5">
         <v>154</v>
       </c>
-      <c r="E46" s="22">
+      <c r="E46" s="23">
         <v>77</v>
       </c>
     </row>
@@ -2031,13 +2032,13 @@
       <c r="A47" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="22">
+      <c r="B47" s="23">
         <v>75</v>
       </c>
-      <c r="C47" s="22">
+      <c r="C47" s="23">
         <v>94</v>
       </c>
-      <c r="D47" s="22">
+      <c r="D47" s="23">
         <v>107</v>
       </c>
       <c r="E47" s="5">
@@ -2048,16 +2049,16 @@
       <c r="A48" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="22">
+      <c r="B48" s="23">
         <v>109</v>
       </c>
       <c r="C48" s="5">
         <v>145</v>
       </c>
-      <c r="D48" s="22">
+      <c r="D48" s="23">
         <v>119</v>
       </c>
-      <c r="E48" s="22">
+      <c r="E48" s="23">
         <v>126</v>
       </c>
     </row>
@@ -2065,13 +2066,13 @@
       <c r="A49" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="22">
+      <c r="B49" s="23">
         <v>107</v>
       </c>
-      <c r="C49" s="22">
+      <c r="C49" s="23">
         <v>115</v>
       </c>
-      <c r="D49" s="22">
+      <c r="D49" s="23">
         <v>102</v>
       </c>
       <c r="E49" s="5">
@@ -2082,13 +2083,13 @@
       <c r="A50" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="22">
+      <c r="B50" s="23">
         <v>93</v>
       </c>
-      <c r="C50" s="22">
+      <c r="C50" s="23">
         <v>118</v>
       </c>
-      <c r="D50" s="22">
+      <c r="D50" s="23">
         <v>85</v>
       </c>
       <c r="E50" s="5">
@@ -2096,22 +2097,22 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="19">
-        <v>45577</v>
-      </c>
-      <c r="B51" s="20">
+      <c r="A51" s="20">
+        <v>45584</v>
+      </c>
+      <c r="B51" s="21">
         <f>AVERAGE(B52:B57)</f>
         <v>107.666666666667</v>
       </c>
-      <c r="C51" s="24">
+      <c r="C51" s="25">
         <f>AVERAGE(C52:C57)</f>
         <v>139.166666666667</v>
       </c>
-      <c r="D51" s="20">
+      <c r="D51" s="21">
         <f>AVERAGE(D52:D57)</f>
         <v>111.5</v>
       </c>
-      <c r="E51" s="23">
+      <c r="E51" s="24">
         <f>AVERAGE(E52:E57)</f>
         <v>109</v>
       </c>
@@ -2120,16 +2121,16 @@
       <c r="A52" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B52" s="25">
+      <c r="B52" s="23">
         <v>106</v>
       </c>
       <c r="C52" s="5">
         <v>157</v>
       </c>
-      <c r="D52" s="26">
+      <c r="D52" s="23">
         <v>102</v>
       </c>
-      <c r="E52" s="25">
+      <c r="E52" s="23">
         <v>132</v>
       </c>
     </row>
@@ -2137,16 +2138,16 @@
       <c r="A53" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="25">
+      <c r="B53" s="23">
         <v>136</v>
       </c>
       <c r="C53" s="5">
         <v>144</v>
       </c>
-      <c r="D53" s="26">
+      <c r="D53" s="23">
         <v>97</v>
       </c>
-      <c r="E53" s="25">
+      <c r="E53" s="23">
         <v>88</v>
       </c>
     </row>
@@ -2154,16 +2155,16 @@
       <c r="A54" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B54" s="25">
+      <c r="B54" s="23">
         <v>96</v>
       </c>
-      <c r="C54" s="25">
+      <c r="C54" s="23">
         <v>122</v>
       </c>
       <c r="D54" s="5">
         <v>136</v>
       </c>
-      <c r="E54" s="26">
+      <c r="E54" s="23">
         <v>108</v>
       </c>
     </row>
@@ -2171,16 +2172,16 @@
       <c r="A55" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B55" s="25">
+      <c r="B55" s="23">
         <v>83</v>
       </c>
       <c r="C55" s="5">
         <v>141</v>
       </c>
-      <c r="D55" s="25">
+      <c r="D55" s="23">
         <v>88</v>
       </c>
-      <c r="E55" s="25">
+      <c r="E55" s="23">
         <v>109</v>
       </c>
     </row>
@@ -2191,13 +2192,13 @@
       <c r="B56" s="5">
         <v>133</v>
       </c>
-      <c r="C56" s="25">
+      <c r="C56" s="23">
         <v>111</v>
       </c>
-      <c r="D56" s="25">
+      <c r="D56" s="23">
         <v>108</v>
       </c>
-      <c r="E56" s="26">
+      <c r="E56" s="23">
         <v>107</v>
       </c>
     </row>
@@ -2205,17 +2206,123 @@
       <c r="A57" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B57" s="25">
+      <c r="B57" s="23">
         <v>92</v>
       </c>
       <c r="C57" s="5">
         <v>160</v>
       </c>
-      <c r="D57" s="25">
+      <c r="D57" s="23">
         <v>138</v>
       </c>
-      <c r="E57" s="26">
+      <c r="E57" s="23">
         <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="20">
+        <v>45668</v>
+      </c>
+      <c r="B58" s="21">
+        <f>AVERAGE(B59:B63)</f>
+        <v>113</v>
+      </c>
+      <c r="C58" s="25">
+        <f>AVERAGE(C59:C63)</f>
+        <v>123</v>
+      </c>
+      <c r="D58" s="21">
+        <f>AVERAGE(D59:D63)</f>
+        <v>105.6</v>
+      </c>
+      <c r="E58" s="24">
+        <f>AVERAGE(E59:E63)</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="5">
+        <v>146</v>
+      </c>
+      <c r="C59" s="26">
+        <v>123</v>
+      </c>
+      <c r="D59" s="27">
+        <v>114</v>
+      </c>
+      <c r="E59" s="27">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" s="5">
+        <v>141</v>
+      </c>
+      <c r="C60" s="26">
+        <v>139</v>
+      </c>
+      <c r="D60" s="27">
+        <v>106</v>
+      </c>
+      <c r="E60" s="27">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="27">
+        <v>89</v>
+      </c>
+      <c r="C61" s="5">
+        <v>125</v>
+      </c>
+      <c r="D61" s="26">
+        <v>112</v>
+      </c>
+      <c r="E61" s="27">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" s="27">
+        <v>102</v>
+      </c>
+      <c r="C62" s="5">
+        <v>112</v>
+      </c>
+      <c r="D62" s="27">
+        <v>81</v>
+      </c>
+      <c r="E62" s="27">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" s="26">
+        <v>87</v>
+      </c>
+      <c r="C63" s="27">
+        <v>116</v>
+      </c>
+      <c r="D63" s="27">
+        <v>115</v>
+      </c>
+      <c r="E63" s="5">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2230,7 +2337,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -2281,7 +2388,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2">
         <v>4</v>
@@ -2293,11 +2400,11 @@
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2">
         <f>SUM(4*C2,3*D2,2*E2,1*F2,G2)</f>
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" ht="25" customHeight="1" spans="1:8">
@@ -2317,14 +2424,14 @@
         <v>3</v>
       </c>
       <c r="F3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="2">
         <f>SUM(4*C3,3*D3,2*E3,1*F3,G3)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" ht="25" customHeight="1" spans="1:8">
@@ -2341,7 +2448,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
@@ -2351,7 +2458,7 @@
       </c>
       <c r="H4" s="2">
         <f>SUM(4*C4,3*D4,2*E4,1*F4,G4)</f>
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" ht="27" customHeight="1" spans="1:8">
@@ -2365,7 +2472,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
@@ -2374,11 +2481,11 @@
         <v>6</v>
       </c>
       <c r="G5" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H5" s="2">
         <f>SUM(4*C5,3*D5,2*E5,1*F5,G5)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2">

</xml_diff>